<commit_message>
fel drug misdem 5 yrs computed
</commit_message>
<xml_diff>
--- a/NOTES/Features Table Notes.xlsx
+++ b/NOTES/Features Table Notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b75526bde7fdd30/Duke/Criminal Recidivism/crim-recid-code/NOTES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caroline Wang\OneDrive\Duke\Criminal Recidivism\crim-recid-code\NOTES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="35" documentId="EB0C0D87C3A5455C3FE76A0BB9FB976926820A50" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{C11048FA-0C07-4B67-916C-DC78611CF70C}"/>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06112D43-9546-4FEC-A272-922A8E136E69}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>